<commit_message>
Updated BOM & added PCB mounting holes in tray
</commit_message>
<xml_diff>
--- a/System_development/Jocassee/V0.6.0/PCB/V0.6.3/PCB V0.6.3 BOM.xlsx
+++ b/System_development/Jocassee/V0.6.0/PCB/V0.6.3/PCB V0.6.3 BOM.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARTS Lab projects\In-situ Water monitor\In-Situ-Water-Quality-Sensor\System_development\Jocassee\V0.6.0\PCB\V0.6.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495CB5FA-ED4A-4FB1-85BC-D2E4DB8A432D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86122AAE-2FD4-444D-9B6B-D9984D3CFDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F872AE6-6710-4898-8598-9832416C0361}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB V0.6.3 BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>Qty</t>
   </si>
@@ -151,9 +164,6 @@
     <t>160/220 ohm resistor</t>
   </si>
   <si>
-    <t>Net cost</t>
-  </si>
-  <si>
     <t>PCB Reference</t>
   </si>
   <si>
@@ -166,18 +176,12 @@
     <t>Unit cost (USD)</t>
   </si>
   <si>
-    <t>2N2222A/BC337 BJT</t>
-  </si>
-  <si>
     <t>AMS1117 3.3v regulator SOT-223-3L</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>2s Lipo battery 7.4V</t>
-  </si>
-  <si>
     <t>Waterproof JST Connector</t>
   </si>
   <si>
@@ -185,6 +189,30 @@
   </si>
   <si>
     <t>SMA female to male extension cable</t>
+  </si>
+  <si>
+    <t>2s Lipo battery 7.4V (87 x 33 x 20 mm)</t>
+  </si>
+  <si>
+    <t>Some nice to have items</t>
+  </si>
+  <si>
+    <t>2N2222A/BC337 BJT or equivalent</t>
+  </si>
+  <si>
+    <t>40 pin Female header connector 2.54mm</t>
+  </si>
+  <si>
+    <t>40 pin Male header connector 2.54mm</t>
+  </si>
+  <si>
+    <t>USB to serial converter module</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Net cost (USD)</t>
   </si>
 </sst>
 </file>
@@ -335,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,8 +549,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -652,6 +686,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -698,7 +745,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -707,9 +754,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -722,6 +766,19 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1098,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7FF72E9-9057-43B3-9849-7848ED564DB8}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,425 +1167,593 @@
     <col min="2" max="2" width="35.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>43</v>
+      <c r="D1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>2</v>
       </c>
       <c r="D2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>0.59</v>
+      </c>
+      <c r="E2" s="3">
+        <f>PRODUCT(C2,D2)</f>
+        <v>1.18</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="3">
         <v>0.31</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E27" si="0">PRODUCT(C3,D3)</f>
+        <v>0.31</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" s="3">
         <v>0.18</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5" s="3">
         <v>0.26</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.26</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>3</v>
       </c>
       <c r="D6" s="3">
         <v>0.19</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>0.57000000000000006</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>2</v>
       </c>
       <c r="D7" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>4.8499999999999996</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10" s="3">
         <v>2.54</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>2.54</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="4">
         <v>1</v>
       </c>
       <c r="D11" s="3">
         <v>0.22</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>0.22</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>1</v>
       </c>
       <c r="D12" s="3">
         <v>0.1</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>2</v>
       </c>
       <c r="D13" s="3">
         <v>0.1</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>1</v>
       </c>
       <c r="D14" s="3">
         <v>0.1</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>2</v>
       </c>
       <c r="D15" s="3">
         <v>0.1</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>2</v>
       </c>
       <c r="D16" s="3">
         <v>0.1</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="C17" s="4">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>1</v>
       </c>
       <c r="D18" s="3">
         <v>19.5</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>19.5</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>1</v>
       </c>
       <c r="D19" s="3">
         <v>45.99</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>45.99</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>1</v>
       </c>
       <c r="D20" s="3">
         <v>67.989999999999995</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>67.989999999999995</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="B21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="5">
-        <v>1</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="C23" s="4">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2.95</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>2.95</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="B24" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="4">
         <v>1</v>
       </c>
       <c r="D24" s="3">
         <v>0.63</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>0.63</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="5">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="4">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3">
+        <v>5</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="5">
-        <v>1</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3">
+        <v>40</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="4">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="14">
+        <f>SUM(E2:E27)</f>
+        <v>218.25</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="A29" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="B30" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E30" s="3">
+        <f>PRODUCT(C30,D30)</f>
+        <v>1.0900000000000001</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="B31" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="4">
+        <v>1</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1.59</v>
+      </c>
+      <c r="E31" s="3">
+        <f t="shared" ref="E31:E32" si="1">PRODUCT(C31,D31)</f>
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" s="13">
+        <f>SUM(E30:E32)</f>
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A29:E29"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{64E976B5-24C5-4081-9712-F007CF32C5F0}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{B10459D7-58B8-4F51-84AF-D90FBABE58DB}"/>
@@ -1537,7 +1762,7 @@
     <hyperlink ref="B6" r:id="rId5" xr:uid="{6E063A02-5BAF-4412-9080-E7006F26C9EE}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{3630D0B1-0861-4C0E-9759-F1A7CB0ED988}"/>
     <hyperlink ref="B10" r:id="rId7" xr:uid="{5F9659A5-436C-405F-95EB-131015CF00F0}"/>
-    <hyperlink ref="B11" r:id="rId8" xr:uid="{CD9201BB-6D8B-47E4-9C13-DD060FB3E831}"/>
+    <hyperlink ref="B11" r:id="rId8" display="2N2222A/BC337 BJT" xr:uid="{CD9201BB-6D8B-47E4-9C13-DD060FB3E831}"/>
     <hyperlink ref="B12" r:id="rId9" xr:uid="{967B8B79-7E91-45DA-B563-628E625FCABB}"/>
     <hyperlink ref="B13" r:id="rId10" xr:uid="{48863A9B-B0E4-465F-92F8-8FE44159BD94}"/>
     <hyperlink ref="B14" r:id="rId11" xr:uid="{5028FF20-8E3F-4E42-9BE6-F7801D7C6492}"/>
@@ -1547,8 +1772,20 @@
     <hyperlink ref="B19" r:id="rId15" xr:uid="{3A9E83BE-009C-424C-95E0-84A920DD0057}"/>
     <hyperlink ref="B20" r:id="rId16" xr:uid="{9DA28E99-0953-4FD6-8932-B280CC55FA73}"/>
     <hyperlink ref="B18" r:id="rId17" xr:uid="{C3CC9103-59D0-4834-8130-5074A5C4222D}"/>
+    <hyperlink ref="B17" r:id="rId18" xr:uid="{B47927C9-FDCD-4982-99BF-FD15F1332E58}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{FAA869AF-43F7-4086-A641-EC1685848DAC}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{6EC27CE5-7F20-4B94-91D0-61D94911B326}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{B951D90F-141D-4675-A649-F9B3713515FC}"/>
+    <hyperlink ref="B8" r:id="rId22" xr:uid="{FFF0089E-2DB9-461C-9641-00C675E56D0E}"/>
+    <hyperlink ref="B25" r:id="rId23" xr:uid="{6E511095-3B86-4545-BA0D-E811909F1290}"/>
+    <hyperlink ref="B27" r:id="rId24" xr:uid="{54ADA80F-C64D-434D-BFD6-662AA69294C0}"/>
+    <hyperlink ref="B9" r:id="rId25" xr:uid="{ABEF0709-956B-4156-A0D4-66EEF675B50C}"/>
+    <hyperlink ref="B26" r:id="rId26" xr:uid="{AA1D0AE0-2996-4749-A21E-EFF9E3238A6E}"/>
+    <hyperlink ref="B31" r:id="rId27" xr:uid="{76F82EF6-C09F-432C-9144-36D146528C3E}"/>
+    <hyperlink ref="B30" r:id="rId28" xr:uid="{2054B9D8-0DC1-4FDB-9925-3B0E696C099E}"/>
+    <hyperlink ref="B32" r:id="rId29" xr:uid="{F26A0CC9-11E5-4FF9-8EE7-7A8A79D860A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solar panels added in BOM, Buy now have holes for wires
</commit_message>
<xml_diff>
--- a/System_development/Jocassee/V0.6.0/PCB/V0.6.3/PCB V0.6.3 BOM.xlsx
+++ b/System_development/Jocassee/V0.6.0/PCB/V0.6.3/PCB V0.6.3 BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARTS Lab projects\In-situ Water monitor\In-Situ-Water-Quality-Sensor\System_development\Jocassee\V0.6.0\PCB\V0.6.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86122AAE-2FD4-444D-9B6B-D9984D3CFDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0C4A2D-DE3C-419C-A3C7-5FC0153C7DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F872AE6-6710-4898-8598-9832416C0361}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Qty</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Net cost (USD)</t>
+  </si>
+  <si>
+    <t>Solar panels</t>
   </si>
 </sst>
 </file>
@@ -693,9 +696,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -745,7 +746,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -766,18 +767,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -1155,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7FF72E9-9057-43B3-9849-7848ED564DB8}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1219,7 +1213,7 @@
         <v>0.31</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E27" si="0">PRODUCT(C3,D3)</f>
+        <f t="shared" ref="E3:E28" si="0">PRODUCT(C3,D3)</f>
         <v>0.31</v>
       </c>
     </row>
@@ -1656,103 +1650,101 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="8" t="s">
+      <c r="A28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="4">
+        <v>9</v>
+      </c>
+      <c r="D28" s="3">
+        <v>7.39</v>
+      </c>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>66.509999999999991</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="14">
-        <f>SUM(E2:E27)</f>
-        <v>218.25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
+      <c r="E29" s="11">
+        <f>SUM(E2:E28)</f>
+        <v>284.76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="4">
-        <v>1</v>
-      </c>
-      <c r="D30" s="3">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="E30" s="3">
-        <f>PRODUCT(C30,D30)</f>
-        <v>1.0900000000000001</v>
-      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="4">
         <v>1</v>
       </c>
       <c r="D31" s="3">
-        <v>1.59</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="E31" s="3">
-        <f t="shared" ref="E31:E32" si="1">PRODUCT(C31,D31)</f>
-        <v>1.59</v>
+        <f>PRODUCT(C31,D31)</f>
+        <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1.59</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" ref="E32:E33" si="1">PRODUCT(C32,D32)</f>
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="4">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3">
+      <c r="C33" s="4">
+        <v>1</v>
+      </c>
+      <c r="D33" s="3">
         <v>6.5</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E33" s="3">
         <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="3" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D34" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E33" s="13">
-        <f>SUM(E30:E32)</f>
+      <c r="E34" s="8">
+        <f>SUM(E31:E33)</f>
         <v>9.18</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A30:E30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{64E976B5-24C5-4081-9712-F007CF32C5F0}"/>
@@ -1781,11 +1773,12 @@
     <hyperlink ref="B27" r:id="rId24" xr:uid="{54ADA80F-C64D-434D-BFD6-662AA69294C0}"/>
     <hyperlink ref="B9" r:id="rId25" xr:uid="{ABEF0709-956B-4156-A0D4-66EEF675B50C}"/>
     <hyperlink ref="B26" r:id="rId26" xr:uid="{AA1D0AE0-2996-4749-A21E-EFF9E3238A6E}"/>
-    <hyperlink ref="B31" r:id="rId27" xr:uid="{76F82EF6-C09F-432C-9144-36D146528C3E}"/>
-    <hyperlink ref="B30" r:id="rId28" xr:uid="{2054B9D8-0DC1-4FDB-9925-3B0E696C099E}"/>
-    <hyperlink ref="B32" r:id="rId29" xr:uid="{F26A0CC9-11E5-4FF9-8EE7-7A8A79D860A2}"/>
+    <hyperlink ref="B32" r:id="rId27" xr:uid="{76F82EF6-C09F-432C-9144-36D146528C3E}"/>
+    <hyperlink ref="B31" r:id="rId28" xr:uid="{2054B9D8-0DC1-4FDB-9925-3B0E696C099E}"/>
+    <hyperlink ref="B33" r:id="rId29" xr:uid="{F26A0CC9-11E5-4FF9-8EE7-7A8A79D860A2}"/>
+    <hyperlink ref="B28" r:id="rId30" xr:uid="{D3C57C8B-2EF7-4A02-BD02-006B33D9B567}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
replaced Amazon parts with eBay
</commit_message>
<xml_diff>
--- a/System_development/Jocassee/V0.6.0/PCB/V0.6.3/PCB V0.6.3 BOM.xlsx
+++ b/System_development/Jocassee/V0.6.0/PCB/V0.6.3/PCB V0.6.3 BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARTS Lab projects\In-situ Water monitor\In-Situ-Water-Quality-Sensor\System_development\Jocassee\V0.6.0\PCB\V0.6.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0C4A2D-DE3C-419C-A3C7-5FC0153C7DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7558D3DB-9F41-4CFE-815E-2934F178E9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F872AE6-6710-4898-8598-9832416C0361}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
   <si>
     <t>Qty</t>
   </si>
@@ -216,13 +216,25 @@
   </si>
   <si>
     <t>Solar panels</t>
+  </si>
+  <si>
+    <t>mouser</t>
+  </si>
+  <si>
+    <t>digikey</t>
+  </si>
+  <si>
+    <t>atlas</t>
+  </si>
+  <si>
+    <t>eBay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,8 +377,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -556,6 +575,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC1F0C8"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -746,7 +783,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -768,11 +805,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1149,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7FF72E9-9057-43B3-9849-7848ED564DB8}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,7 +1206,7 @@
     <col min="5" max="5" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
@@ -1181,7 +1223,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1198,8 +1240,11 @@
         <f>PRODUCT(C2,D2)</f>
         <v>1.18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1216,8 +1261,11 @@
         <f t="shared" ref="E3:E28" si="0">PRODUCT(C3,D3)</f>
         <v>0.31</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
@@ -1234,8 +1282,11 @@
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
@@ -1252,8 +1303,11 @@
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -1270,8 +1324,11 @@
         <f t="shared" si="0"/>
         <v>0.57000000000000006</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -1288,8 +1345,11 @@
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1306,8 +1366,11 @@
         <f t="shared" si="0"/>
         <v>4.8499999999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1318,14 +1381,17 @@
         <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>10</v>
+        <v>10.65</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10.65</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1342,8 +1408,11 @@
         <f t="shared" si="0"/>
         <v>2.54</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1360,8 +1429,11 @@
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1378,8 +1450,11 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -1396,8 +1471,11 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -1414,8 +1492,11 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1432,8 +1513,11 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1450,8 +1534,11 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -1462,14 +1549,17 @@
         <v>1</v>
       </c>
       <c r="D17" s="3">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E17" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.5</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -1486,8 +1576,11 @@
         <f t="shared" si="0"/>
         <v>19.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1504,8 +1597,11 @@
         <f t="shared" si="0"/>
         <v>45.99</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1522,8 +1618,11 @@
         <f t="shared" si="0"/>
         <v>67.989999999999995</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -1534,14 +1633,17 @@
         <v>1</v>
       </c>
       <c r="D21" s="3">
-        <v>2.5</v>
+        <v>1.87</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.87</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -1552,14 +1654,17 @@
         <v>1</v>
       </c>
       <c r="D22" s="3">
-        <v>3.5</v>
+        <v>1.76</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.76</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -1576,8 +1681,11 @@
         <f t="shared" si="0"/>
         <v>2.95</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -1594,8 +1702,11 @@
         <f t="shared" si="0"/>
         <v>0.63</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -1606,14 +1717,17 @@
         <v>1</v>
       </c>
       <c r="D25" s="3">
-        <v>5</v>
+        <v>8.2799999999999994</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
@@ -1624,14 +1738,17 @@
         <v>1</v>
       </c>
       <c r="D26" s="3">
-        <v>40</v>
+        <v>59.59</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59.59</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>48</v>
       </c>
@@ -1642,14 +1759,17 @@
         <v>2</v>
       </c>
       <c r="D27" s="3">
-        <v>2</v>
+        <v>2.58</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.16</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>48</v>
       </c>
@@ -1666,26 +1786,31 @@
         <f t="shared" si="0"/>
         <v>66.509999999999991</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D29" s="10" t="s">
+      <c r="F28" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D29" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="10">
         <f>SUM(E2:E28)</f>
-        <v>284.76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+        <v>304.56999999999994</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="6" t="s">
         <v>55</v>
@@ -1700,8 +1825,11 @@
         <f>PRODUCT(C31,D31)</f>
         <v>1.0900000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="6" t="s">
         <v>56</v>
@@ -1716,8 +1844,11 @@
         <f t="shared" ref="E32:E33" si="1">PRODUCT(C32,D32)</f>
         <v>1.59</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="6" t="s">
         <v>57</v>
@@ -1726,20 +1857,23 @@
         <v>1</v>
       </c>
       <c r="D33" s="3">
-        <v>6.5</v>
+        <v>2.75</v>
       </c>
       <c r="E33" s="3">
         <f t="shared" si="1"/>
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.75</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D34" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E34" s="8">
         <f>SUM(E31:E33)</f>
-        <v>9.18</v>
+        <v>5.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Src price changed to USD only
</commit_message>
<xml_diff>
--- a/System_development/Jocassee/V0.6.0/PCB/V0.6.3/PCB V0.6.3 BOM.xlsx
+++ b/System_development/Jocassee/V0.6.0/PCB/V0.6.3/PCB V0.6.3 BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ARTS Lab projects\In-situ Water monitor\In-Situ-Water-Quality-Sensor\System_development\Jocassee\V0.6.0\PCB\V0.6.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7558D3DB-9F41-4CFE-815E-2934F178E9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAD90AF-B76C-4777-88B4-F69CA39B465C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3F872AE6-6710-4898-8598-9832416C0361}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
   <si>
     <t>Qty</t>
   </si>
@@ -218,9 +218,6 @@
     <t>Solar panels</t>
   </si>
   <si>
-    <t>mouser</t>
-  </si>
-  <si>
     <t>digikey</t>
   </si>
   <si>
@@ -228,6 +225,18 @@
   </si>
   <si>
     <t>eBay</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have </t>
+  </si>
+  <si>
+    <t>Sells two in a lot.</t>
   </si>
 </sst>
 </file>
@@ -385,7 +394,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,12 +584,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
@@ -783,7 +786,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -804,17 +807,18 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1191,10 +1195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7FF72E9-9057-43B3-9849-7848ED564DB8}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1204,9 +1208,10 @@
     <col min="3" max="3" width="7.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.109375" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>43</v>
       </c>
@@ -1222,8 +1227,14 @@
       <c r="E1" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1240,11 +1251,12 @@
         <f>PRODUCT(C2,D2)</f>
         <v>1.18</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1261,11 +1273,12 @@
         <f t="shared" ref="E3:E28" si="0">PRODUCT(C3,D3)</f>
         <v>0.31</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
@@ -1282,11 +1295,14 @@
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
@@ -1303,11 +1319,14 @@
         <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -1324,11 +1343,12 @@
         <f t="shared" si="0"/>
         <v>0.57000000000000006</v>
       </c>
-      <c r="F6" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -1345,11 +1365,12 @@
         <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="F7" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1366,11 +1387,14 @@
         <f t="shared" si="0"/>
         <v>4.8499999999999996</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1381,17 +1405,18 @@
         <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>10.65</v>
+        <v>12.74</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>10.65</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12.74</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1408,11 +1433,12 @@
         <f t="shared" si="0"/>
         <v>2.54</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
@@ -1429,11 +1455,12 @@
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1450,11 +1477,12 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -1471,11 +1499,12 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
@@ -1492,11 +1521,12 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F14" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
@@ -1513,11 +1543,12 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="F15" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
@@ -1534,11 +1565,12 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="F16" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F16" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -1555,11 +1587,12 @@
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
@@ -1576,11 +1609,12 @@
         <f t="shared" si="0"/>
         <v>19.5</v>
       </c>
-      <c r="F18" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1597,11 +1631,12 @@
         <f t="shared" si="0"/>
         <v>45.99</v>
       </c>
-      <c r="F19" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
@@ -1618,11 +1653,12 @@
         <f t="shared" si="0"/>
         <v>67.989999999999995</v>
       </c>
-      <c r="F20" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
@@ -1633,17 +1669,18 @@
         <v>1</v>
       </c>
       <c r="D21" s="3">
-        <v>1.87</v>
+        <v>1.85</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" si="0"/>
-        <v>1.87</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1.85</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -1654,17 +1691,18 @@
         <v>1</v>
       </c>
       <c r="D22" s="3">
-        <v>1.76</v>
+        <v>2.15</v>
       </c>
       <c r="E22" s="3">
         <f t="shared" si="0"/>
-        <v>1.76</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2.15</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -1675,17 +1713,18 @@
         <v>1</v>
       </c>
       <c r="D23" s="3">
-        <v>2.95</v>
+        <v>3.5</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" si="0"/>
-        <v>2.95</v>
-      </c>
-      <c r="F23" s="12" t="s">
+        <v>3.5</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -1702,11 +1741,12 @@
         <f t="shared" si="0"/>
         <v>0.63</v>
       </c>
-      <c r="F24" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F24" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -1723,11 +1763,14 @@
         <f t="shared" si="0"/>
         <v>8.2799999999999994</v>
       </c>
-      <c r="F25" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F25" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
@@ -1738,17 +1781,20 @@
         <v>1</v>
       </c>
       <c r="D26" s="3">
-        <v>59.59</v>
+        <v>11.7</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" si="0"/>
-        <v>59.59</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11.7</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>48</v>
       </c>
@@ -1765,11 +1811,12 @@
         <f t="shared" si="0"/>
         <v>5.16</v>
       </c>
-      <c r="F27" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F27" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>48</v>
       </c>
@@ -1786,31 +1833,34 @@
         <f t="shared" si="0"/>
         <v>66.509999999999991</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D29" s="9" t="s">
+      <c r="F28" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D29" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="9">
         <f>SUM(E2:E28)</f>
-        <v>304.56999999999994</v>
+        <v>259.68999999999994</v>
       </c>
       <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
       <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="6" t="s">
         <v>55</v>
@@ -1826,10 +1876,11 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="6" t="s">
         <v>56</v>
@@ -1845,10 +1896,11 @@
         <v>1.59</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="6" t="s">
         <v>57</v>
@@ -1863,15 +1915,16 @@
         <f t="shared" si="1"/>
         <v>2.75</v>
       </c>
-      <c r="F33" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F33" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D34" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="14">
         <f>SUM(E31:E33)</f>
         <v>5.43</v>
       </c>

</xml_diff>